<commit_message>
Add example 10 with internal checking capabilities
</commit_message>
<xml_diff>
--- a/ampl-data-input-excel/10-PM.Daniel/10-PM.Daniel.xlsx
+++ b/ampl-data-input-excel/10-PM.Daniel/10-PM.Daniel.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="9"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="experts" sheetId="1" state="visible" r:id="rId3"/>
@@ -625,9 +625,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="@"/>
-    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
-    <numFmt numFmtId="167" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+    <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+    <numFmt numFmtId="166" formatCode="@"/>
+    <numFmt numFmtId="167" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
   <fonts count="10">
     <font>
@@ -752,7 +752,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -761,7 +761,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -769,15 +769,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -789,7 +789,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -797,31 +797,31 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -829,15 +829,11 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -845,11 +841,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1036,10 +1032,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:D1015"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1269,37 +1265,2997 @@
       <c r="D21" s="1"/>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C22" s="6"/>
       <c r="D22" s="1"/>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C23" s="6"/>
       <c r="D23" s="1"/>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C24" s="6"/>
       <c r="D24" s="1"/>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C25" s="6"/>
       <c r="D25" s="1"/>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C26" s="6"/>
       <c r="D26" s="1"/>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C27" s="6"/>
       <c r="D27" s="1"/>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C28" s="6"/>
       <c r="D28" s="1"/>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C29" s="6"/>
       <c r="D29" s="1"/>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C30" s="6"/>
       <c r="D30" s="1"/>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C31" s="6"/>
       <c r="D31" s="1"/>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C32" s="6"/>
       <c r="D32" s="1"/>
+    </row>
+    <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C33" s="6"/>
+    </row>
+    <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C34" s="6"/>
+    </row>
+    <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C35" s="6"/>
+    </row>
+    <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C36" s="6"/>
+    </row>
+    <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C37" s="6"/>
+    </row>
+    <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C38" s="6"/>
+    </row>
+    <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C39" s="6"/>
+    </row>
+    <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C40" s="6"/>
+    </row>
+    <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C41" s="6"/>
+    </row>
+    <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C42" s="6"/>
+    </row>
+    <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C43" s="6"/>
+    </row>
+    <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C44" s="6"/>
+    </row>
+    <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C45" s="6"/>
+    </row>
+    <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C46" s="6"/>
+    </row>
+    <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C47" s="6"/>
+    </row>
+    <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C48" s="6"/>
+    </row>
+    <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C49" s="6"/>
+    </row>
+    <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C50" s="6"/>
+    </row>
+    <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C51" s="6"/>
+    </row>
+    <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C52" s="6"/>
+    </row>
+    <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C53" s="6"/>
+    </row>
+    <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C54" s="6"/>
+    </row>
+    <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C55" s="6"/>
+    </row>
+    <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C56" s="6"/>
+    </row>
+    <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C57" s="6"/>
+    </row>
+    <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C58" s="6"/>
+    </row>
+    <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C59" s="6"/>
+    </row>
+    <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C60" s="6"/>
+    </row>
+    <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C61" s="6"/>
+    </row>
+    <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C62" s="6"/>
+    </row>
+    <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C63" s="6"/>
+    </row>
+    <row r="64" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C64" s="6"/>
+    </row>
+    <row r="65" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C65" s="6"/>
+    </row>
+    <row r="66" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C66" s="6"/>
+    </row>
+    <row r="67" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C67" s="6"/>
+    </row>
+    <row r="68" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C68" s="6"/>
+    </row>
+    <row r="69" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C69" s="6"/>
+    </row>
+    <row r="70" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C70" s="6"/>
+    </row>
+    <row r="71" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C71" s="6"/>
+    </row>
+    <row r="72" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C72" s="6"/>
+    </row>
+    <row r="73" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C73" s="6"/>
+    </row>
+    <row r="74" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C74" s="6"/>
+    </row>
+    <row r="75" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C75" s="6"/>
+    </row>
+    <row r="76" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C76" s="6"/>
+    </row>
+    <row r="77" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C77" s="6"/>
+    </row>
+    <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C78" s="6"/>
+    </row>
+    <row r="79" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C79" s="6"/>
+    </row>
+    <row r="80" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C80" s="6"/>
+    </row>
+    <row r="81" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C81" s="6"/>
+    </row>
+    <row r="82" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C82" s="6"/>
+    </row>
+    <row r="83" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C83" s="6"/>
+    </row>
+    <row r="84" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C84" s="6"/>
+    </row>
+    <row r="85" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C85" s="6"/>
+    </row>
+    <row r="86" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C86" s="6"/>
+    </row>
+    <row r="87" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C87" s="6"/>
+    </row>
+    <row r="88" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C88" s="6"/>
+    </row>
+    <row r="89" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C89" s="6"/>
+    </row>
+    <row r="90" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C90" s="6"/>
+    </row>
+    <row r="91" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C91" s="6"/>
+    </row>
+    <row r="92" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C92" s="6"/>
+    </row>
+    <row r="93" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C93" s="6"/>
+    </row>
+    <row r="94" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C94" s="6"/>
+    </row>
+    <row r="95" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C95" s="6"/>
+    </row>
+    <row r="96" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C96" s="6"/>
+    </row>
+    <row r="97" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C97" s="6"/>
+    </row>
+    <row r="98" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C98" s="6"/>
+    </row>
+    <row r="99" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C99" s="6"/>
+    </row>
+    <row r="100" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C100" s="6"/>
+    </row>
+    <row r="101" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C101" s="6"/>
+    </row>
+    <row r="102" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C102" s="6"/>
+    </row>
+    <row r="103" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C103" s="6"/>
+    </row>
+    <row r="104" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C104" s="6"/>
+    </row>
+    <row r="105" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C105" s="6"/>
+    </row>
+    <row r="106" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C106" s="6"/>
+    </row>
+    <row r="107" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C107" s="6"/>
+    </row>
+    <row r="108" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C108" s="6"/>
+    </row>
+    <row r="109" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C109" s="6"/>
+    </row>
+    <row r="110" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C110" s="6"/>
+    </row>
+    <row r="111" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C111" s="6"/>
+    </row>
+    <row r="112" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C112" s="6"/>
+    </row>
+    <row r="113" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C113" s="6"/>
+    </row>
+    <row r="114" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C114" s="6"/>
+    </row>
+    <row r="115" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C115" s="6"/>
+    </row>
+    <row r="116" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C116" s="6"/>
+    </row>
+    <row r="117" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C117" s="6"/>
+    </row>
+    <row r="118" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C118" s="6"/>
+    </row>
+    <row r="119" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C119" s="6"/>
+    </row>
+    <row r="120" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C120" s="6"/>
+    </row>
+    <row r="121" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C121" s="6"/>
+    </row>
+    <row r="122" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C122" s="6"/>
+    </row>
+    <row r="123" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C123" s="6"/>
+    </row>
+    <row r="124" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C124" s="6"/>
+    </row>
+    <row r="125" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C125" s="6"/>
+    </row>
+    <row r="126" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C126" s="6"/>
+    </row>
+    <row r="127" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C127" s="6"/>
+    </row>
+    <row r="128" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C128" s="6"/>
+    </row>
+    <row r="129" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C129" s="6"/>
+    </row>
+    <row r="130" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C130" s="6"/>
+    </row>
+    <row r="131" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C131" s="6"/>
+    </row>
+    <row r="132" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C132" s="6"/>
+    </row>
+    <row r="133" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C133" s="6"/>
+    </row>
+    <row r="134" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C134" s="6"/>
+    </row>
+    <row r="135" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C135" s="6"/>
+    </row>
+    <row r="136" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C136" s="6"/>
+    </row>
+    <row r="137" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C137" s="6"/>
+    </row>
+    <row r="138" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C138" s="6"/>
+    </row>
+    <row r="139" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C139" s="6"/>
+    </row>
+    <row r="140" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C140" s="6"/>
+    </row>
+    <row r="141" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C141" s="6"/>
+    </row>
+    <row r="142" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C142" s="6"/>
+    </row>
+    <row r="143" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C143" s="6"/>
+    </row>
+    <row r="144" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C144" s="6"/>
+    </row>
+    <row r="145" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C145" s="6"/>
+    </row>
+    <row r="146" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C146" s="6"/>
+    </row>
+    <row r="147" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C147" s="6"/>
+    </row>
+    <row r="148" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C148" s="6"/>
+    </row>
+    <row r="149" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C149" s="6"/>
+    </row>
+    <row r="150" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C150" s="6"/>
+    </row>
+    <row r="151" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C151" s="6"/>
+    </row>
+    <row r="152" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C152" s="6"/>
+    </row>
+    <row r="153" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C153" s="6"/>
+    </row>
+    <row r="154" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C154" s="6"/>
+    </row>
+    <row r="155" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C155" s="6"/>
+    </row>
+    <row r="156" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C156" s="6"/>
+    </row>
+    <row r="157" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C157" s="6"/>
+    </row>
+    <row r="158" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C158" s="6"/>
+    </row>
+    <row r="159" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C159" s="6"/>
+    </row>
+    <row r="160" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C160" s="6"/>
+    </row>
+    <row r="161" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C161" s="6"/>
+    </row>
+    <row r="162" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C162" s="6"/>
+    </row>
+    <row r="163" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C163" s="6"/>
+    </row>
+    <row r="164" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C164" s="6"/>
+    </row>
+    <row r="165" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C165" s="6"/>
+    </row>
+    <row r="166" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C166" s="6"/>
+    </row>
+    <row r="167" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C167" s="6"/>
+    </row>
+    <row r="168" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C168" s="6"/>
+    </row>
+    <row r="169" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C169" s="6"/>
+    </row>
+    <row r="170" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C170" s="6"/>
+    </row>
+    <row r="171" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C171" s="6"/>
+    </row>
+    <row r="172" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C172" s="6"/>
+    </row>
+    <row r="173" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C173" s="6"/>
+    </row>
+    <row r="174" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C174" s="6"/>
+    </row>
+    <row r="175" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C175" s="6"/>
+    </row>
+    <row r="176" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C176" s="6"/>
+    </row>
+    <row r="177" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C177" s="6"/>
+    </row>
+    <row r="178" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C178" s="6"/>
+    </row>
+    <row r="179" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C179" s="6"/>
+    </row>
+    <row r="180" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C180" s="6"/>
+    </row>
+    <row r="181" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C181" s="6"/>
+    </row>
+    <row r="182" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C182" s="6"/>
+    </row>
+    <row r="183" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C183" s="6"/>
+    </row>
+    <row r="184" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C184" s="6"/>
+    </row>
+    <row r="185" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C185" s="6"/>
+    </row>
+    <row r="186" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C186" s="6"/>
+    </row>
+    <row r="187" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C187" s="6"/>
+    </row>
+    <row r="188" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C188" s="6"/>
+    </row>
+    <row r="189" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C189" s="6"/>
+    </row>
+    <row r="190" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C190" s="6"/>
+    </row>
+    <row r="191" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C191" s="6"/>
+    </row>
+    <row r="192" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C192" s="6"/>
+    </row>
+    <row r="193" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C193" s="6"/>
+    </row>
+    <row r="194" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C194" s="6"/>
+    </row>
+    <row r="195" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C195" s="6"/>
+    </row>
+    <row r="196" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C196" s="6"/>
+    </row>
+    <row r="197" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C197" s="6"/>
+    </row>
+    <row r="198" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C198" s="6"/>
+    </row>
+    <row r="199" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C199" s="6"/>
+    </row>
+    <row r="200" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C200" s="6"/>
+    </row>
+    <row r="201" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C201" s="6"/>
+    </row>
+    <row r="202" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C202" s="6"/>
+    </row>
+    <row r="203" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C203" s="6"/>
+    </row>
+    <row r="204" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C204" s="6"/>
+    </row>
+    <row r="205" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C205" s="6"/>
+    </row>
+    <row r="206" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C206" s="6"/>
+    </row>
+    <row r="207" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C207" s="6"/>
+    </row>
+    <row r="208" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C208" s="6"/>
+    </row>
+    <row r="209" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C209" s="6"/>
+    </row>
+    <row r="210" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C210" s="6"/>
+    </row>
+    <row r="211" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C211" s="6"/>
+    </row>
+    <row r="212" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C212" s="6"/>
+    </row>
+    <row r="213" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C213" s="6"/>
+    </row>
+    <row r="214" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C214" s="6"/>
+    </row>
+    <row r="215" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C215" s="6"/>
+    </row>
+    <row r="216" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C216" s="6"/>
+    </row>
+    <row r="217" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C217" s="6"/>
+    </row>
+    <row r="218" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C218" s="6"/>
+    </row>
+    <row r="219" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C219" s="6"/>
+    </row>
+    <row r="220" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C220" s="6"/>
+    </row>
+    <row r="221" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C221" s="6"/>
+    </row>
+    <row r="222" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C222" s="6"/>
+    </row>
+    <row r="223" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C223" s="6"/>
+    </row>
+    <row r="224" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C224" s="6"/>
+    </row>
+    <row r="225" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C225" s="6"/>
+    </row>
+    <row r="226" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C226" s="6"/>
+    </row>
+    <row r="227" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C227" s="6"/>
+    </row>
+    <row r="228" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C228" s="6"/>
+    </row>
+    <row r="229" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C229" s="6"/>
+    </row>
+    <row r="230" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C230" s="6"/>
+    </row>
+    <row r="231" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C231" s="6"/>
+    </row>
+    <row r="232" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C232" s="6"/>
+    </row>
+    <row r="233" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C233" s="6"/>
+    </row>
+    <row r="234" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C234" s="6"/>
+    </row>
+    <row r="235" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C235" s="6"/>
+    </row>
+    <row r="236" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C236" s="6"/>
+    </row>
+    <row r="237" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C237" s="6"/>
+    </row>
+    <row r="238" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C238" s="6"/>
+    </row>
+    <row r="239" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C239" s="6"/>
+    </row>
+    <row r="240" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C240" s="6"/>
+    </row>
+    <row r="241" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C241" s="6"/>
+    </row>
+    <row r="242" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C242" s="6"/>
+    </row>
+    <row r="243" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C243" s="6"/>
+    </row>
+    <row r="244" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C244" s="6"/>
+    </row>
+    <row r="245" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C245" s="6"/>
+    </row>
+    <row r="246" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C246" s="6"/>
+    </row>
+    <row r="247" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C247" s="6"/>
+    </row>
+    <row r="248" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C248" s="6"/>
+    </row>
+    <row r="249" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C249" s="6"/>
+    </row>
+    <row r="250" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C250" s="6"/>
+    </row>
+    <row r="251" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C251" s="6"/>
+    </row>
+    <row r="252" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C252" s="6"/>
+    </row>
+    <row r="253" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C253" s="6"/>
+    </row>
+    <row r="254" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C254" s="6"/>
+    </row>
+    <row r="255" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C255" s="6"/>
+    </row>
+    <row r="256" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C256" s="6"/>
+    </row>
+    <row r="257" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C257" s="6"/>
+    </row>
+    <row r="258" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C258" s="6"/>
+    </row>
+    <row r="259" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C259" s="6"/>
+    </row>
+    <row r="260" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C260" s="6"/>
+    </row>
+    <row r="261" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C261" s="6"/>
+    </row>
+    <row r="262" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C262" s="6"/>
+    </row>
+    <row r="263" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C263" s="6"/>
+    </row>
+    <row r="264" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C264" s="6"/>
+    </row>
+    <row r="265" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C265" s="6"/>
+    </row>
+    <row r="266" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C266" s="6"/>
+    </row>
+    <row r="267" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C267" s="6"/>
+    </row>
+    <row r="268" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C268" s="6"/>
+    </row>
+    <row r="269" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C269" s="6"/>
+    </row>
+    <row r="270" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C270" s="6"/>
+    </row>
+    <row r="271" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C271" s="6"/>
+    </row>
+    <row r="272" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C272" s="6"/>
+    </row>
+    <row r="273" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C273" s="6"/>
+    </row>
+    <row r="274" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C274" s="6"/>
+    </row>
+    <row r="275" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C275" s="6"/>
+    </row>
+    <row r="276" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C276" s="6"/>
+    </row>
+    <row r="277" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C277" s="6"/>
+    </row>
+    <row r="278" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C278" s="6"/>
+    </row>
+    <row r="279" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C279" s="6"/>
+    </row>
+    <row r="280" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C280" s="6"/>
+    </row>
+    <row r="281" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C281" s="6"/>
+    </row>
+    <row r="282" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C282" s="6"/>
+    </row>
+    <row r="283" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C283" s="6"/>
+    </row>
+    <row r="284" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C284" s="6"/>
+    </row>
+    <row r="285" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C285" s="6"/>
+    </row>
+    <row r="286" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C286" s="6"/>
+    </row>
+    <row r="287" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C287" s="6"/>
+    </row>
+    <row r="288" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C288" s="6"/>
+    </row>
+    <row r="289" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C289" s="6"/>
+    </row>
+    <row r="290" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C290" s="6"/>
+    </row>
+    <row r="291" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C291" s="6"/>
+    </row>
+    <row r="292" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C292" s="6"/>
+    </row>
+    <row r="293" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C293" s="6"/>
+    </row>
+    <row r="294" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C294" s="6"/>
+    </row>
+    <row r="295" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C295" s="6"/>
+    </row>
+    <row r="296" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C296" s="6"/>
+    </row>
+    <row r="297" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C297" s="6"/>
+    </row>
+    <row r="298" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C298" s="6"/>
+    </row>
+    <row r="299" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C299" s="6"/>
+    </row>
+    <row r="300" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C300" s="6"/>
+    </row>
+    <row r="301" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C301" s="6"/>
+    </row>
+    <row r="302" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C302" s="6"/>
+    </row>
+    <row r="303" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C303" s="6"/>
+    </row>
+    <row r="304" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C304" s="6"/>
+    </row>
+    <row r="305" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C305" s="6"/>
+    </row>
+    <row r="306" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C306" s="6"/>
+    </row>
+    <row r="307" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C307" s="6"/>
+    </row>
+    <row r="308" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C308" s="6"/>
+    </row>
+    <row r="309" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C309" s="6"/>
+    </row>
+    <row r="310" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C310" s="6"/>
+    </row>
+    <row r="311" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C311" s="6"/>
+    </row>
+    <row r="312" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C312" s="6"/>
+    </row>
+    <row r="313" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C313" s="6"/>
+    </row>
+    <row r="314" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C314" s="6"/>
+    </row>
+    <row r="315" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C315" s="6"/>
+    </row>
+    <row r="316" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C316" s="6"/>
+    </row>
+    <row r="317" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C317" s="6"/>
+    </row>
+    <row r="318" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C318" s="6"/>
+    </row>
+    <row r="319" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C319" s="6"/>
+    </row>
+    <row r="320" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C320" s="6"/>
+    </row>
+    <row r="321" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C321" s="6"/>
+    </row>
+    <row r="322" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C322" s="6"/>
+    </row>
+    <row r="323" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C323" s="6"/>
+    </row>
+    <row r="324" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C324" s="6"/>
+    </row>
+    <row r="325" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C325" s="6"/>
+    </row>
+    <row r="326" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C326" s="6"/>
+    </row>
+    <row r="327" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C327" s="6"/>
+    </row>
+    <row r="328" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C328" s="6"/>
+    </row>
+    <row r="329" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C329" s="6"/>
+    </row>
+    <row r="330" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C330" s="6"/>
+    </row>
+    <row r="331" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C331" s="6"/>
+    </row>
+    <row r="332" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C332" s="6"/>
+    </row>
+    <row r="333" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C333" s="6"/>
+    </row>
+    <row r="334" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C334" s="6"/>
+    </row>
+    <row r="335" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C335" s="6"/>
+    </row>
+    <row r="336" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C336" s="6"/>
+    </row>
+    <row r="337" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C337" s="6"/>
+    </row>
+    <row r="338" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C338" s="6"/>
+    </row>
+    <row r="339" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C339" s="6"/>
+    </row>
+    <row r="340" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C340" s="6"/>
+    </row>
+    <row r="341" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C341" s="6"/>
+    </row>
+    <row r="342" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C342" s="6"/>
+    </row>
+    <row r="343" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C343" s="6"/>
+    </row>
+    <row r="344" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C344" s="6"/>
+    </row>
+    <row r="345" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C345" s="6"/>
+    </row>
+    <row r="346" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C346" s="6"/>
+    </row>
+    <row r="347" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C347" s="6"/>
+    </row>
+    <row r="348" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C348" s="6"/>
+    </row>
+    <row r="349" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C349" s="6"/>
+    </row>
+    <row r="350" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C350" s="6"/>
+    </row>
+    <row r="351" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C351" s="6"/>
+    </row>
+    <row r="352" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C352" s="6"/>
+    </row>
+    <row r="353" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C353" s="6"/>
+    </row>
+    <row r="354" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C354" s="6"/>
+    </row>
+    <row r="355" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C355" s="6"/>
+    </row>
+    <row r="356" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C356" s="6"/>
+    </row>
+    <row r="357" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C357" s="6"/>
+    </row>
+    <row r="358" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C358" s="6"/>
+    </row>
+    <row r="359" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C359" s="6"/>
+    </row>
+    <row r="360" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C360" s="6"/>
+    </row>
+    <row r="361" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C361" s="6"/>
+    </row>
+    <row r="362" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C362" s="6"/>
+    </row>
+    <row r="363" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C363" s="6"/>
+    </row>
+    <row r="364" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C364" s="6"/>
+    </row>
+    <row r="365" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C365" s="6"/>
+    </row>
+    <row r="366" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C366" s="6"/>
+    </row>
+    <row r="367" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C367" s="6"/>
+    </row>
+    <row r="368" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C368" s="6"/>
+    </row>
+    <row r="369" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C369" s="6"/>
+    </row>
+    <row r="370" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C370" s="6"/>
+    </row>
+    <row r="371" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C371" s="6"/>
+    </row>
+    <row r="372" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C372" s="6"/>
+    </row>
+    <row r="373" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C373" s="6"/>
+    </row>
+    <row r="374" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C374" s="6"/>
+    </row>
+    <row r="375" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C375" s="6"/>
+    </row>
+    <row r="376" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C376" s="6"/>
+    </row>
+    <row r="377" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C377" s="6"/>
+    </row>
+    <row r="378" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C378" s="6"/>
+    </row>
+    <row r="379" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C379" s="6"/>
+    </row>
+    <row r="380" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C380" s="6"/>
+    </row>
+    <row r="381" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C381" s="6"/>
+    </row>
+    <row r="382" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C382" s="6"/>
+    </row>
+    <row r="383" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C383" s="6"/>
+    </row>
+    <row r="384" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C384" s="6"/>
+    </row>
+    <row r="385" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C385" s="6"/>
+    </row>
+    <row r="386" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C386" s="6"/>
+    </row>
+    <row r="387" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C387" s="6"/>
+    </row>
+    <row r="388" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C388" s="6"/>
+    </row>
+    <row r="389" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C389" s="6"/>
+    </row>
+    <row r="390" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C390" s="6"/>
+    </row>
+    <row r="391" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C391" s="6"/>
+    </row>
+    <row r="392" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C392" s="6"/>
+    </row>
+    <row r="393" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C393" s="6"/>
+    </row>
+    <row r="394" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C394" s="6"/>
+    </row>
+    <row r="395" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C395" s="6"/>
+    </row>
+    <row r="396" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C396" s="6"/>
+    </row>
+    <row r="397" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C397" s="6"/>
+    </row>
+    <row r="398" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C398" s="6"/>
+    </row>
+    <row r="399" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C399" s="6"/>
+    </row>
+    <row r="400" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C400" s="6"/>
+    </row>
+    <row r="401" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C401" s="6"/>
+    </row>
+    <row r="402" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C402" s="6"/>
+    </row>
+    <row r="403" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C403" s="6"/>
+    </row>
+    <row r="404" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C404" s="6"/>
+    </row>
+    <row r="405" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C405" s="6"/>
+    </row>
+    <row r="406" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C406" s="6"/>
+    </row>
+    <row r="407" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C407" s="6"/>
+    </row>
+    <row r="408" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C408" s="6"/>
+    </row>
+    <row r="409" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C409" s="6"/>
+    </row>
+    <row r="410" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C410" s="6"/>
+    </row>
+    <row r="411" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C411" s="6"/>
+    </row>
+    <row r="412" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C412" s="6"/>
+    </row>
+    <row r="413" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C413" s="6"/>
+    </row>
+    <row r="414" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C414" s="6"/>
+    </row>
+    <row r="415" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C415" s="6"/>
+    </row>
+    <row r="416" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C416" s="6"/>
+    </row>
+    <row r="417" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C417" s="6"/>
+    </row>
+    <row r="418" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C418" s="6"/>
+    </row>
+    <row r="419" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C419" s="6"/>
+    </row>
+    <row r="420" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C420" s="6"/>
+    </row>
+    <row r="421" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C421" s="6"/>
+    </row>
+    <row r="422" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C422" s="6"/>
+    </row>
+    <row r="423" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C423" s="6"/>
+    </row>
+    <row r="424" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C424" s="6"/>
+    </row>
+    <row r="425" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C425" s="6"/>
+    </row>
+    <row r="426" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C426" s="6"/>
+    </row>
+    <row r="427" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C427" s="6"/>
+    </row>
+    <row r="428" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C428" s="6"/>
+    </row>
+    <row r="429" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C429" s="6"/>
+    </row>
+    <row r="430" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C430" s="6"/>
+    </row>
+    <row r="431" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C431" s="6"/>
+    </row>
+    <row r="432" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C432" s="6"/>
+    </row>
+    <row r="433" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C433" s="6"/>
+    </row>
+    <row r="434" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C434" s="6"/>
+    </row>
+    <row r="435" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C435" s="6"/>
+    </row>
+    <row r="436" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C436" s="6"/>
+    </row>
+    <row r="437" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C437" s="6"/>
+    </row>
+    <row r="438" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C438" s="6"/>
+    </row>
+    <row r="439" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C439" s="6"/>
+    </row>
+    <row r="440" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C440" s="6"/>
+    </row>
+    <row r="441" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C441" s="6"/>
+    </row>
+    <row r="442" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C442" s="6"/>
+    </row>
+    <row r="443" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C443" s="6"/>
+    </row>
+    <row r="444" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C444" s="6"/>
+    </row>
+    <row r="445" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C445" s="6"/>
+    </row>
+    <row r="446" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C446" s="6"/>
+    </row>
+    <row r="447" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C447" s="6"/>
+    </row>
+    <row r="448" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C448" s="6"/>
+    </row>
+    <row r="449" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C449" s="6"/>
+    </row>
+    <row r="450" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C450" s="6"/>
+    </row>
+    <row r="451" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C451" s="6"/>
+    </row>
+    <row r="452" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C452" s="6"/>
+    </row>
+    <row r="453" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C453" s="6"/>
+    </row>
+    <row r="454" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C454" s="6"/>
+    </row>
+    <row r="455" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C455" s="6"/>
+    </row>
+    <row r="456" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C456" s="6"/>
+    </row>
+    <row r="457" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C457" s="6"/>
+    </row>
+    <row r="458" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C458" s="6"/>
+    </row>
+    <row r="459" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C459" s="6"/>
+    </row>
+    <row r="460" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C460" s="6"/>
+    </row>
+    <row r="461" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C461" s="6"/>
+    </row>
+    <row r="462" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C462" s="6"/>
+    </row>
+    <row r="463" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C463" s="6"/>
+    </row>
+    <row r="464" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C464" s="6"/>
+    </row>
+    <row r="465" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C465" s="6"/>
+    </row>
+    <row r="466" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C466" s="6"/>
+    </row>
+    <row r="467" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C467" s="6"/>
+    </row>
+    <row r="468" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C468" s="6"/>
+    </row>
+    <row r="469" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C469" s="6"/>
+    </row>
+    <row r="470" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C470" s="6"/>
+    </row>
+    <row r="471" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C471" s="6"/>
+    </row>
+    <row r="472" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C472" s="6"/>
+    </row>
+    <row r="473" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C473" s="6"/>
+    </row>
+    <row r="474" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C474" s="6"/>
+    </row>
+    <row r="475" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C475" s="6"/>
+    </row>
+    <row r="476" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C476" s="6"/>
+    </row>
+    <row r="477" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C477" s="6"/>
+    </row>
+    <row r="478" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C478" s="6"/>
+    </row>
+    <row r="479" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C479" s="6"/>
+    </row>
+    <row r="480" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C480" s="6"/>
+    </row>
+    <row r="481" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C481" s="6"/>
+    </row>
+    <row r="482" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C482" s="6"/>
+    </row>
+    <row r="483" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C483" s="6"/>
+    </row>
+    <row r="484" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C484" s="6"/>
+    </row>
+    <row r="485" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C485" s="6"/>
+    </row>
+    <row r="486" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C486" s="6"/>
+    </row>
+    <row r="487" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C487" s="6"/>
+    </row>
+    <row r="488" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C488" s="6"/>
+    </row>
+    <row r="489" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C489" s="6"/>
+    </row>
+    <row r="490" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C490" s="6"/>
+    </row>
+    <row r="491" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C491" s="6"/>
+    </row>
+    <row r="492" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C492" s="6"/>
+    </row>
+    <row r="493" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C493" s="6"/>
+    </row>
+    <row r="494" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C494" s="6"/>
+    </row>
+    <row r="495" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C495" s="6"/>
+    </row>
+    <row r="496" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C496" s="6"/>
+    </row>
+    <row r="497" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C497" s="6"/>
+    </row>
+    <row r="498" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C498" s="6"/>
+    </row>
+    <row r="499" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C499" s="6"/>
+    </row>
+    <row r="500" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C500" s="6"/>
+    </row>
+    <row r="501" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C501" s="6"/>
+    </row>
+    <row r="502" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C502" s="6"/>
+    </row>
+    <row r="503" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C503" s="6"/>
+    </row>
+    <row r="504" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C504" s="6"/>
+    </row>
+    <row r="505" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C505" s="6"/>
+    </row>
+    <row r="506" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C506" s="6"/>
+    </row>
+    <row r="507" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C507" s="6"/>
+    </row>
+    <row r="508" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C508" s="6"/>
+    </row>
+    <row r="509" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C509" s="6"/>
+    </row>
+    <row r="510" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C510" s="6"/>
+    </row>
+    <row r="511" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C511" s="6"/>
+    </row>
+    <row r="512" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C512" s="6"/>
+    </row>
+    <row r="513" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C513" s="6"/>
+    </row>
+    <row r="514" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C514" s="6"/>
+    </row>
+    <row r="515" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C515" s="6"/>
+    </row>
+    <row r="516" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C516" s="6"/>
+    </row>
+    <row r="517" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C517" s="6"/>
+    </row>
+    <row r="518" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C518" s="6"/>
+    </row>
+    <row r="519" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C519" s="6"/>
+    </row>
+    <row r="520" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C520" s="6"/>
+    </row>
+    <row r="521" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C521" s="6"/>
+    </row>
+    <row r="522" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C522" s="6"/>
+    </row>
+    <row r="523" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C523" s="6"/>
+    </row>
+    <row r="524" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C524" s="6"/>
+    </row>
+    <row r="525" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C525" s="6"/>
+    </row>
+    <row r="526" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C526" s="6"/>
+    </row>
+    <row r="527" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C527" s="6"/>
+    </row>
+    <row r="528" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C528" s="6"/>
+    </row>
+    <row r="529" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C529" s="6"/>
+    </row>
+    <row r="530" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C530" s="6"/>
+    </row>
+    <row r="531" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C531" s="6"/>
+    </row>
+    <row r="532" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C532" s="6"/>
+    </row>
+    <row r="533" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C533" s="6"/>
+    </row>
+    <row r="534" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C534" s="6"/>
+    </row>
+    <row r="535" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C535" s="6"/>
+    </row>
+    <row r="536" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C536" s="6"/>
+    </row>
+    <row r="537" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C537" s="6"/>
+    </row>
+    <row r="538" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C538" s="6"/>
+    </row>
+    <row r="539" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C539" s="6"/>
+    </row>
+    <row r="540" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C540" s="6"/>
+    </row>
+    <row r="541" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C541" s="6"/>
+    </row>
+    <row r="542" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C542" s="6"/>
+    </row>
+    <row r="543" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C543" s="6"/>
+    </row>
+    <row r="544" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C544" s="6"/>
+    </row>
+    <row r="545" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C545" s="6"/>
+    </row>
+    <row r="546" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C546" s="6"/>
+    </row>
+    <row r="547" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C547" s="6"/>
+    </row>
+    <row r="548" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C548" s="6"/>
+    </row>
+    <row r="549" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C549" s="6"/>
+    </row>
+    <row r="550" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C550" s="6"/>
+    </row>
+    <row r="551" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C551" s="6"/>
+    </row>
+    <row r="552" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C552" s="6"/>
+    </row>
+    <row r="553" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C553" s="6"/>
+    </row>
+    <row r="554" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C554" s="6"/>
+    </row>
+    <row r="555" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C555" s="6"/>
+    </row>
+    <row r="556" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C556" s="6"/>
+    </row>
+    <row r="557" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C557" s="6"/>
+    </row>
+    <row r="558" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C558" s="6"/>
+    </row>
+    <row r="559" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C559" s="6"/>
+    </row>
+    <row r="560" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C560" s="6"/>
+    </row>
+    <row r="561" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C561" s="6"/>
+    </row>
+    <row r="562" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C562" s="6"/>
+    </row>
+    <row r="563" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C563" s="6"/>
+    </row>
+    <row r="564" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C564" s="6"/>
+    </row>
+    <row r="565" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C565" s="6"/>
+    </row>
+    <row r="566" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C566" s="6"/>
+    </row>
+    <row r="567" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C567" s="6"/>
+    </row>
+    <row r="568" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C568" s="6"/>
+    </row>
+    <row r="569" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C569" s="6"/>
+    </row>
+    <row r="570" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C570" s="6"/>
+    </row>
+    <row r="571" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C571" s="6"/>
+    </row>
+    <row r="572" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C572" s="6"/>
+    </row>
+    <row r="573" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C573" s="6"/>
+    </row>
+    <row r="574" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C574" s="6"/>
+    </row>
+    <row r="575" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C575" s="6"/>
+    </row>
+    <row r="576" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C576" s="6"/>
+    </row>
+    <row r="577" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C577" s="6"/>
+    </row>
+    <row r="578" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C578" s="6"/>
+    </row>
+    <row r="579" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C579" s="6"/>
+    </row>
+    <row r="580" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C580" s="6"/>
+    </row>
+    <row r="581" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C581" s="6"/>
+    </row>
+    <row r="582" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C582" s="6"/>
+    </row>
+    <row r="583" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C583" s="6"/>
+    </row>
+    <row r="584" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C584" s="6"/>
+    </row>
+    <row r="585" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C585" s="6"/>
+    </row>
+    <row r="586" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C586" s="6"/>
+    </row>
+    <row r="587" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C587" s="6"/>
+    </row>
+    <row r="588" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C588" s="6"/>
+    </row>
+    <row r="589" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C589" s="6"/>
+    </row>
+    <row r="590" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C590" s="6"/>
+    </row>
+    <row r="591" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C591" s="6"/>
+    </row>
+    <row r="592" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C592" s="6"/>
+    </row>
+    <row r="593" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C593" s="6"/>
+    </row>
+    <row r="594" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C594" s="6"/>
+    </row>
+    <row r="595" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C595" s="6"/>
+    </row>
+    <row r="596" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C596" s="6"/>
+    </row>
+    <row r="597" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C597" s="6"/>
+    </row>
+    <row r="598" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C598" s="6"/>
+    </row>
+    <row r="599" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C599" s="6"/>
+    </row>
+    <row r="600" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C600" s="6"/>
+    </row>
+    <row r="601" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C601" s="6"/>
+    </row>
+    <row r="602" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C602" s="6"/>
+    </row>
+    <row r="603" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C603" s="6"/>
+    </row>
+    <row r="604" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C604" s="6"/>
+    </row>
+    <row r="605" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C605" s="6"/>
+    </row>
+    <row r="606" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C606" s="6"/>
+    </row>
+    <row r="607" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C607" s="6"/>
+    </row>
+    <row r="608" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C608" s="6"/>
+    </row>
+    <row r="609" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C609" s="6"/>
+    </row>
+    <row r="610" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C610" s="6"/>
+    </row>
+    <row r="611" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C611" s="6"/>
+    </row>
+    <row r="612" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C612" s="6"/>
+    </row>
+    <row r="613" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C613" s="6"/>
+    </row>
+    <row r="614" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C614" s="6"/>
+    </row>
+    <row r="615" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C615" s="6"/>
+    </row>
+    <row r="616" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C616" s="6"/>
+    </row>
+    <row r="617" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C617" s="6"/>
+    </row>
+    <row r="618" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C618" s="6"/>
+    </row>
+    <row r="619" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C619" s="6"/>
+    </row>
+    <row r="620" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C620" s="6"/>
+    </row>
+    <row r="621" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C621" s="6"/>
+    </row>
+    <row r="622" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C622" s="6"/>
+    </row>
+    <row r="623" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C623" s="6"/>
+    </row>
+    <row r="624" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C624" s="6"/>
+    </row>
+    <row r="625" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C625" s="6"/>
+    </row>
+    <row r="626" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C626" s="6"/>
+    </row>
+    <row r="627" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C627" s="6"/>
+    </row>
+    <row r="628" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C628" s="6"/>
+    </row>
+    <row r="629" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C629" s="6"/>
+    </row>
+    <row r="630" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C630" s="6"/>
+    </row>
+    <row r="631" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C631" s="6"/>
+    </row>
+    <row r="632" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C632" s="6"/>
+    </row>
+    <row r="633" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C633" s="6"/>
+    </row>
+    <row r="634" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C634" s="6"/>
+    </row>
+    <row r="635" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C635" s="6"/>
+    </row>
+    <row r="636" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C636" s="6"/>
+    </row>
+    <row r="637" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C637" s="6"/>
+    </row>
+    <row r="638" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C638" s="6"/>
+    </row>
+    <row r="639" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C639" s="6"/>
+    </row>
+    <row r="640" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C640" s="6"/>
+    </row>
+    <row r="641" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C641" s="6"/>
+    </row>
+    <row r="642" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C642" s="6"/>
+    </row>
+    <row r="643" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C643" s="6"/>
+    </row>
+    <row r="644" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C644" s="6"/>
+    </row>
+    <row r="645" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C645" s="6"/>
+    </row>
+    <row r="646" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C646" s="6"/>
+    </row>
+    <row r="647" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C647" s="6"/>
+    </row>
+    <row r="648" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C648" s="6"/>
+    </row>
+    <row r="649" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C649" s="6"/>
+    </row>
+    <row r="650" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C650" s="6"/>
+    </row>
+    <row r="651" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C651" s="6"/>
+    </row>
+    <row r="652" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C652" s="6"/>
+    </row>
+    <row r="653" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C653" s="6"/>
+    </row>
+    <row r="654" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C654" s="6"/>
+    </row>
+    <row r="655" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C655" s="6"/>
+    </row>
+    <row r="656" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C656" s="6"/>
+    </row>
+    <row r="657" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C657" s="6"/>
+    </row>
+    <row r="658" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C658" s="6"/>
+    </row>
+    <row r="659" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C659" s="6"/>
+    </row>
+    <row r="660" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C660" s="6"/>
+    </row>
+    <row r="661" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C661" s="6"/>
+    </row>
+    <row r="662" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C662" s="6"/>
+    </row>
+    <row r="663" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C663" s="6"/>
+    </row>
+    <row r="664" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C664" s="6"/>
+    </row>
+    <row r="665" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C665" s="6"/>
+    </row>
+    <row r="666" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C666" s="6"/>
+    </row>
+    <row r="667" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C667" s="6"/>
+    </row>
+    <row r="668" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C668" s="6"/>
+    </row>
+    <row r="669" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C669" s="6"/>
+    </row>
+    <row r="670" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C670" s="6"/>
+    </row>
+    <row r="671" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C671" s="6"/>
+    </row>
+    <row r="672" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C672" s="6"/>
+    </row>
+    <row r="673" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C673" s="6"/>
+    </row>
+    <row r="674" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C674" s="6"/>
+    </row>
+    <row r="675" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C675" s="6"/>
+    </row>
+    <row r="676" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C676" s="6"/>
+    </row>
+    <row r="677" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C677" s="6"/>
+    </row>
+    <row r="678" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C678" s="6"/>
+    </row>
+    <row r="679" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C679" s="6"/>
+    </row>
+    <row r="680" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C680" s="6"/>
+    </row>
+    <row r="681" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C681" s="6"/>
+    </row>
+    <row r="682" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C682" s="6"/>
+    </row>
+    <row r="683" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C683" s="6"/>
+    </row>
+    <row r="684" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C684" s="6"/>
+    </row>
+    <row r="685" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C685" s="6"/>
+    </row>
+    <row r="686" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C686" s="6"/>
+    </row>
+    <row r="687" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C687" s="6"/>
+    </row>
+    <row r="688" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C688" s="6"/>
+    </row>
+    <row r="689" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C689" s="6"/>
+    </row>
+    <row r="690" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C690" s="6"/>
+    </row>
+    <row r="691" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C691" s="6"/>
+    </row>
+    <row r="692" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C692" s="6"/>
+    </row>
+    <row r="693" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C693" s="6"/>
+    </row>
+    <row r="694" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C694" s="6"/>
+    </row>
+    <row r="695" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C695" s="6"/>
+    </row>
+    <row r="696" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C696" s="6"/>
+    </row>
+    <row r="697" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C697" s="6"/>
+    </row>
+    <row r="698" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C698" s="6"/>
+    </row>
+    <row r="699" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C699" s="6"/>
+    </row>
+    <row r="700" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C700" s="6"/>
+    </row>
+    <row r="701" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C701" s="6"/>
+    </row>
+    <row r="702" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C702" s="6"/>
+    </row>
+    <row r="703" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C703" s="6"/>
+    </row>
+    <row r="704" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C704" s="6"/>
+    </row>
+    <row r="705" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C705" s="6"/>
+    </row>
+    <row r="706" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C706" s="6"/>
+    </row>
+    <row r="707" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C707" s="6"/>
+    </row>
+    <row r="708" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C708" s="6"/>
+    </row>
+    <row r="709" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C709" s="6"/>
+    </row>
+    <row r="710" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C710" s="6"/>
+    </row>
+    <row r="711" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C711" s="6"/>
+    </row>
+    <row r="712" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C712" s="6"/>
+    </row>
+    <row r="713" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C713" s="6"/>
+    </row>
+    <row r="714" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C714" s="6"/>
+    </row>
+    <row r="715" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C715" s="6"/>
+    </row>
+    <row r="716" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C716" s="6"/>
+    </row>
+    <row r="717" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C717" s="6"/>
+    </row>
+    <row r="718" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C718" s="6"/>
+    </row>
+    <row r="719" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C719" s="6"/>
+    </row>
+    <row r="720" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C720" s="6"/>
+    </row>
+    <row r="721" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C721" s="6"/>
+    </row>
+    <row r="722" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C722" s="6"/>
+    </row>
+    <row r="723" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C723" s="6"/>
+    </row>
+    <row r="724" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C724" s="6"/>
+    </row>
+    <row r="725" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C725" s="6"/>
+    </row>
+    <row r="726" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C726" s="6"/>
+    </row>
+    <row r="727" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C727" s="6"/>
+    </row>
+    <row r="728" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C728" s="6"/>
+    </row>
+    <row r="729" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C729" s="6"/>
+    </row>
+    <row r="730" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C730" s="6"/>
+    </row>
+    <row r="731" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C731" s="6"/>
+    </row>
+    <row r="732" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C732" s="6"/>
+    </row>
+    <row r="733" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C733" s="6"/>
+    </row>
+    <row r="734" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C734" s="6"/>
+    </row>
+    <row r="735" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C735" s="6"/>
+    </row>
+    <row r="736" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C736" s="6"/>
+    </row>
+    <row r="737" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C737" s="6"/>
+    </row>
+    <row r="738" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C738" s="6"/>
+    </row>
+    <row r="739" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C739" s="6"/>
+    </row>
+    <row r="740" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C740" s="6"/>
+    </row>
+    <row r="741" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C741" s="6"/>
+    </row>
+    <row r="742" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C742" s="6"/>
+    </row>
+    <row r="743" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C743" s="6"/>
+    </row>
+    <row r="744" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C744" s="6"/>
+    </row>
+    <row r="745" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C745" s="6"/>
+    </row>
+    <row r="746" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C746" s="6"/>
+    </row>
+    <row r="747" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C747" s="6"/>
+    </row>
+    <row r="748" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C748" s="6"/>
+    </row>
+    <row r="749" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C749" s="6"/>
+    </row>
+    <row r="750" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C750" s="6"/>
+    </row>
+    <row r="751" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C751" s="6"/>
+    </row>
+    <row r="752" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C752" s="6"/>
+    </row>
+    <row r="753" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C753" s="6"/>
+    </row>
+    <row r="754" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C754" s="6"/>
+    </row>
+    <row r="755" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C755" s="6"/>
+    </row>
+    <row r="756" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C756" s="6"/>
+    </row>
+    <row r="757" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C757" s="6"/>
+    </row>
+    <row r="758" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C758" s="6"/>
+    </row>
+    <row r="759" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C759" s="6"/>
+    </row>
+    <row r="760" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C760" s="6"/>
+    </row>
+    <row r="761" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C761" s="6"/>
+    </row>
+    <row r="762" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C762" s="6"/>
+    </row>
+    <row r="763" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C763" s="6"/>
+    </row>
+    <row r="764" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C764" s="6"/>
+    </row>
+    <row r="765" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C765" s="6"/>
+    </row>
+    <row r="766" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C766" s="6"/>
+    </row>
+    <row r="767" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C767" s="6"/>
+    </row>
+    <row r="768" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C768" s="6"/>
+    </row>
+    <row r="769" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C769" s="6"/>
+    </row>
+    <row r="770" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C770" s="6"/>
+    </row>
+    <row r="771" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C771" s="6"/>
+    </row>
+    <row r="772" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C772" s="6"/>
+    </row>
+    <row r="773" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C773" s="6"/>
+    </row>
+    <row r="774" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C774" s="6"/>
+    </row>
+    <row r="775" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C775" s="6"/>
+    </row>
+    <row r="776" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C776" s="6"/>
+    </row>
+    <row r="777" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C777" s="6"/>
+    </row>
+    <row r="778" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C778" s="6"/>
+    </row>
+    <row r="779" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C779" s="6"/>
+    </row>
+    <row r="780" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C780" s="6"/>
+    </row>
+    <row r="781" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C781" s="6"/>
+    </row>
+    <row r="782" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C782" s="6"/>
+    </row>
+    <row r="783" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C783" s="6"/>
+    </row>
+    <row r="784" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C784" s="6"/>
+    </row>
+    <row r="785" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C785" s="6"/>
+    </row>
+    <row r="786" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C786" s="6"/>
+    </row>
+    <row r="787" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C787" s="6"/>
+    </row>
+    <row r="788" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C788" s="6"/>
+    </row>
+    <row r="789" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C789" s="6"/>
+    </row>
+    <row r="790" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C790" s="6"/>
+    </row>
+    <row r="791" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C791" s="6"/>
+    </row>
+    <row r="792" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C792" s="6"/>
+    </row>
+    <row r="793" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C793" s="6"/>
+    </row>
+    <row r="794" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C794" s="6"/>
+    </row>
+    <row r="795" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C795" s="6"/>
+    </row>
+    <row r="796" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C796" s="6"/>
+    </row>
+    <row r="797" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C797" s="6"/>
+    </row>
+    <row r="798" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C798" s="6"/>
+    </row>
+    <row r="799" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C799" s="6"/>
+    </row>
+    <row r="800" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C800" s="6"/>
+    </row>
+    <row r="801" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C801" s="6"/>
+    </row>
+    <row r="802" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C802" s="6"/>
+    </row>
+    <row r="803" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C803" s="6"/>
+    </row>
+    <row r="804" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C804" s="6"/>
+    </row>
+    <row r="805" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C805" s="6"/>
+    </row>
+    <row r="806" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C806" s="6"/>
+    </row>
+    <row r="807" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C807" s="6"/>
+    </row>
+    <row r="808" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C808" s="6"/>
+    </row>
+    <row r="809" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C809" s="6"/>
+    </row>
+    <row r="810" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C810" s="6"/>
+    </row>
+    <row r="811" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C811" s="6"/>
+    </row>
+    <row r="812" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C812" s="6"/>
+    </row>
+    <row r="813" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C813" s="6"/>
+    </row>
+    <row r="814" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C814" s="6"/>
+    </row>
+    <row r="815" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C815" s="6"/>
+    </row>
+    <row r="816" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C816" s="6"/>
+    </row>
+    <row r="817" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C817" s="6"/>
+    </row>
+    <row r="818" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C818" s="6"/>
+    </row>
+    <row r="819" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C819" s="6"/>
+    </row>
+    <row r="820" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C820" s="6"/>
+    </row>
+    <row r="821" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C821" s="6"/>
+    </row>
+    <row r="822" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C822" s="6"/>
+    </row>
+    <row r="823" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C823" s="6"/>
+    </row>
+    <row r="824" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C824" s="6"/>
+    </row>
+    <row r="825" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C825" s="6"/>
+    </row>
+    <row r="826" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C826" s="6"/>
+    </row>
+    <row r="827" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C827" s="6"/>
+    </row>
+    <row r="828" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C828" s="6"/>
+    </row>
+    <row r="829" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C829" s="6"/>
+    </row>
+    <row r="830" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C830" s="6"/>
+    </row>
+    <row r="831" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C831" s="6"/>
+    </row>
+    <row r="832" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C832" s="6"/>
+    </row>
+    <row r="833" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C833" s="6"/>
+    </row>
+    <row r="834" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C834" s="6"/>
+    </row>
+    <row r="835" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C835" s="6"/>
+    </row>
+    <row r="836" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C836" s="6"/>
+    </row>
+    <row r="837" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C837" s="6"/>
+    </row>
+    <row r="838" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C838" s="6"/>
+    </row>
+    <row r="839" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C839" s="6"/>
+    </row>
+    <row r="840" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C840" s="6"/>
+    </row>
+    <row r="841" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C841" s="6"/>
+    </row>
+    <row r="842" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C842" s="6"/>
+    </row>
+    <row r="843" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C843" s="6"/>
+    </row>
+    <row r="844" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C844" s="6"/>
+    </row>
+    <row r="845" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C845" s="6"/>
+    </row>
+    <row r="846" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C846" s="6"/>
+    </row>
+    <row r="847" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C847" s="6"/>
+    </row>
+    <row r="848" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C848" s="6"/>
+    </row>
+    <row r="849" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C849" s="6"/>
+    </row>
+    <row r="850" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C850" s="6"/>
+    </row>
+    <row r="851" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C851" s="6"/>
+    </row>
+    <row r="852" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C852" s="6"/>
+    </row>
+    <row r="853" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C853" s="6"/>
+    </row>
+    <row r="854" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C854" s="6"/>
+    </row>
+    <row r="855" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C855" s="6"/>
+    </row>
+    <row r="856" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C856" s="6"/>
+    </row>
+    <row r="857" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C857" s="6"/>
+    </row>
+    <row r="858" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C858" s="6"/>
+    </row>
+    <row r="859" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C859" s="6"/>
+    </row>
+    <row r="860" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C860" s="6"/>
+    </row>
+    <row r="861" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C861" s="6"/>
+    </row>
+    <row r="862" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C862" s="6"/>
+    </row>
+    <row r="863" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C863" s="6"/>
+    </row>
+    <row r="864" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C864" s="6"/>
+    </row>
+    <row r="865" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C865" s="6"/>
+    </row>
+    <row r="866" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C866" s="6"/>
+    </row>
+    <row r="867" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C867" s="6"/>
+    </row>
+    <row r="868" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C868" s="6"/>
+    </row>
+    <row r="869" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C869" s="6"/>
+    </row>
+    <row r="870" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C870" s="6"/>
+    </row>
+    <row r="871" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C871" s="6"/>
+    </row>
+    <row r="872" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C872" s="6"/>
+    </row>
+    <row r="873" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C873" s="6"/>
+    </row>
+    <row r="874" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C874" s="6"/>
+    </row>
+    <row r="875" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C875" s="6"/>
+    </row>
+    <row r="876" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C876" s="6"/>
+    </row>
+    <row r="877" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C877" s="6"/>
+    </row>
+    <row r="878" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C878" s="6"/>
+    </row>
+    <row r="879" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C879" s="6"/>
+    </row>
+    <row r="880" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C880" s="6"/>
+    </row>
+    <row r="881" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C881" s="6"/>
+    </row>
+    <row r="882" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C882" s="6"/>
+    </row>
+    <row r="883" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C883" s="6"/>
+    </row>
+    <row r="884" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C884" s="6"/>
+    </row>
+    <row r="885" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C885" s="6"/>
+    </row>
+    <row r="886" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C886" s="6"/>
+    </row>
+    <row r="887" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C887" s="6"/>
+    </row>
+    <row r="888" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C888" s="6"/>
+    </row>
+    <row r="889" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C889" s="6"/>
+    </row>
+    <row r="890" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C890" s="6"/>
+    </row>
+    <row r="891" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C891" s="6"/>
+    </row>
+    <row r="892" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C892" s="6"/>
+    </row>
+    <row r="893" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C893" s="6"/>
+    </row>
+    <row r="894" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C894" s="6"/>
+    </row>
+    <row r="895" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C895" s="6"/>
+    </row>
+    <row r="896" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C896" s="6"/>
+    </row>
+    <row r="897" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C897" s="6"/>
+    </row>
+    <row r="898" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C898" s="6"/>
+    </row>
+    <row r="899" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C899" s="6"/>
+    </row>
+    <row r="900" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C900" s="6"/>
+    </row>
+    <row r="901" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C901" s="6"/>
+    </row>
+    <row r="902" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C902" s="6"/>
+    </row>
+    <row r="903" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C903" s="6"/>
+    </row>
+    <row r="904" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C904" s="6"/>
+    </row>
+    <row r="905" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C905" s="6"/>
+    </row>
+    <row r="906" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C906" s="6"/>
+    </row>
+    <row r="907" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C907" s="6"/>
+    </row>
+    <row r="908" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C908" s="6"/>
+    </row>
+    <row r="909" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C909" s="6"/>
+    </row>
+    <row r="910" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C910" s="6"/>
+    </row>
+    <row r="911" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C911" s="6"/>
+    </row>
+    <row r="912" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C912" s="6"/>
+    </row>
+    <row r="913" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C913" s="6"/>
+    </row>
+    <row r="914" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C914" s="6"/>
+    </row>
+    <row r="915" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C915" s="6"/>
+    </row>
+    <row r="916" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C916" s="6"/>
+    </row>
+    <row r="917" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C917" s="6"/>
+    </row>
+    <row r="918" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C918" s="6"/>
+    </row>
+    <row r="919" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C919" s="6"/>
+    </row>
+    <row r="920" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C920" s="6"/>
+    </row>
+    <row r="921" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C921" s="6"/>
+    </row>
+    <row r="922" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C922" s="6"/>
+    </row>
+    <row r="923" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C923" s="6"/>
+    </row>
+    <row r="924" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C924" s="6"/>
+    </row>
+    <row r="925" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C925" s="6"/>
+    </row>
+    <row r="926" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C926" s="6"/>
+    </row>
+    <row r="927" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C927" s="6"/>
+    </row>
+    <row r="928" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C928" s="6"/>
+    </row>
+    <row r="929" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C929" s="6"/>
+    </row>
+    <row r="930" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C930" s="6"/>
+    </row>
+    <row r="931" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C931" s="6"/>
+    </row>
+    <row r="932" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C932" s="6"/>
+    </row>
+    <row r="933" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C933" s="6"/>
+    </row>
+    <row r="934" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C934" s="6"/>
+    </row>
+    <row r="935" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C935" s="6"/>
+    </row>
+    <row r="936" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C936" s="6"/>
+    </row>
+    <row r="937" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C937" s="6"/>
+    </row>
+    <row r="938" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C938" s="6"/>
+    </row>
+    <row r="939" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C939" s="6"/>
+    </row>
+    <row r="940" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C940" s="6"/>
+    </row>
+    <row r="941" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C941" s="6"/>
+    </row>
+    <row r="942" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C942" s="6"/>
+    </row>
+    <row r="943" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C943" s="6"/>
+    </row>
+    <row r="944" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C944" s="6"/>
+    </row>
+    <row r="945" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C945" s="6"/>
+    </row>
+    <row r="946" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C946" s="6"/>
+    </row>
+    <row r="947" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C947" s="6"/>
+    </row>
+    <row r="948" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C948" s="6"/>
+    </row>
+    <row r="949" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C949" s="6"/>
+    </row>
+    <row r="950" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C950" s="6"/>
+    </row>
+    <row r="951" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C951" s="6"/>
+    </row>
+    <row r="952" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C952" s="6"/>
+    </row>
+    <row r="953" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C953" s="6"/>
+    </row>
+    <row r="954" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C954" s="6"/>
+    </row>
+    <row r="955" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C955" s="6"/>
+    </row>
+    <row r="956" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C956" s="6"/>
+    </row>
+    <row r="957" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C957" s="6"/>
+    </row>
+    <row r="958" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C958" s="6"/>
+    </row>
+    <row r="959" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C959" s="6"/>
+    </row>
+    <row r="960" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C960" s="6"/>
+    </row>
+    <row r="961" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C961" s="6"/>
+    </row>
+    <row r="962" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C962" s="6"/>
+    </row>
+    <row r="963" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C963" s="6"/>
+    </row>
+    <row r="964" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C964" s="6"/>
+    </row>
+    <row r="965" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C965" s="6"/>
+    </row>
+    <row r="966" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C966" s="6"/>
+    </row>
+    <row r="967" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C967" s="6"/>
+    </row>
+    <row r="968" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C968" s="6"/>
+    </row>
+    <row r="969" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C969" s="6"/>
+    </row>
+    <row r="970" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C970" s="6"/>
+    </row>
+    <row r="971" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C971" s="6"/>
+    </row>
+    <row r="972" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C972" s="6"/>
+    </row>
+    <row r="973" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C973" s="6"/>
+    </row>
+    <row r="974" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C974" s="6"/>
+    </row>
+    <row r="975" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C975" s="6"/>
+    </row>
+    <row r="976" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C976" s="6"/>
+    </row>
+    <row r="977" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C977" s="6"/>
+    </row>
+    <row r="978" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C978" s="6"/>
+    </row>
+    <row r="979" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C979" s="6"/>
+    </row>
+    <row r="980" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C980" s="6"/>
+    </row>
+    <row r="981" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C981" s="6"/>
+    </row>
+    <row r="982" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C982" s="6"/>
+    </row>
+    <row r="983" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C983" s="6"/>
+    </row>
+    <row r="984" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C984" s="6"/>
+    </row>
+    <row r="985" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C985" s="6"/>
+    </row>
+    <row r="986" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C986" s="6"/>
+    </row>
+    <row r="987" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C987" s="6"/>
+    </row>
+    <row r="988" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C988" s="6"/>
+    </row>
+    <row r="989" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C989" s="6"/>
+    </row>
+    <row r="990" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C990" s="6"/>
+    </row>
+    <row r="991" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C991" s="6"/>
+    </row>
+    <row r="992" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C992" s="6"/>
+    </row>
+    <row r="993" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C993" s="6"/>
+    </row>
+    <row r="994" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C994" s="6"/>
+    </row>
+    <row r="995" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C995" s="6"/>
+    </row>
+    <row r="996" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C996" s="6"/>
+    </row>
+    <row r="997" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C997" s="6"/>
+    </row>
+    <row r="998" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C998" s="6"/>
+    </row>
+    <row r="999" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C999" s="6"/>
+    </row>
+    <row r="1000" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C1000" s="6"/>
+    </row>
+    <row r="1001" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C1001" s="6"/>
+    </row>
+    <row r="1002" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C1002" s="6"/>
+    </row>
+    <row r="1003" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C1003" s="6"/>
+    </row>
+    <row r="1004" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C1004" s="6"/>
+    </row>
+    <row r="1005" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C1005" s="6"/>
+    </row>
+    <row r="1006" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C1006" s="6"/>
+    </row>
+    <row r="1007" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C1007" s="6"/>
+    </row>
+    <row r="1008" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C1008" s="6"/>
+    </row>
+    <row r="1009" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C1009" s="6"/>
+    </row>
+    <row r="1010" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C1010" s="6"/>
+    </row>
+    <row r="1011" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C1011" s="6"/>
+    </row>
+    <row r="1012" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C1012" s="6"/>
+    </row>
+    <row r="1013" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C1013" s="6"/>
+    </row>
+    <row r="1014" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C1014" s="6"/>
+    </row>
+    <row r="1015" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C1015" s="6"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1320,16 +4276,16 @@
   </sheetPr>
   <dimension ref="A1:G169"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H20" activeCellId="0" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="24" width="13.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="23" width="13.71"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="3" style="7" width="11.57"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="11.57"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="6" width="11.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1354,7 +4310,7 @@
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="21" t="s">
         <v>127</v>
       </c>
       <c r="C2" s="1" t="n">
@@ -1373,7 +4329,7 @@
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="21" t="s">
         <v>128</v>
       </c>
       <c r="C3" s="1" t="n">
@@ -1582,7 +4538,7 @@
       <c r="A14" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B14" s="22" t="s">
+      <c r="B14" s="21" t="s">
         <v>127</v>
       </c>
       <c r="C14" s="1" t="n">
@@ -1601,7 +4557,7 @@
       <c r="A15" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="22" t="s">
+      <c r="B15" s="21" t="s">
         <v>128</v>
       </c>
       <c r="C15" s="1" t="n">
@@ -1810,7 +4766,7 @@
       <c r="A26" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B26" s="22" t="s">
+      <c r="B26" s="21" t="s">
         <v>127</v>
       </c>
       <c r="C26" s="1" t="n">
@@ -1829,7 +4785,7 @@
       <c r="A27" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B27" s="22" t="s">
+      <c r="B27" s="21" t="s">
         <v>128</v>
       </c>
       <c r="C27" s="1" t="n">
@@ -2036,7 +4992,7 @@
       <c r="A38" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B38" s="22" t="s">
+      <c r="B38" s="21" t="s">
         <v>127</v>
       </c>
       <c r="C38" s="1" t="n">
@@ -2054,7 +5010,7 @@
       <c r="A39" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B39" s="22" t="s">
+      <c r="B39" s="21" t="s">
         <v>128</v>
       </c>
       <c r="C39" s="1" t="n">
@@ -2252,7 +5208,7 @@
       <c r="A50" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B50" s="22" t="s">
+      <c r="B50" s="21" t="s">
         <v>127</v>
       </c>
       <c r="C50" s="1" t="n">
@@ -2270,7 +5226,7 @@
       <c r="A51" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B51" s="22" t="s">
+      <c r="B51" s="21" t="s">
         <v>128</v>
       </c>
       <c r="C51" s="1" t="n">
@@ -2472,7 +5428,7 @@
       <c r="A62" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B62" s="22" t="s">
+      <c r="B62" s="21" t="s">
         <v>127</v>
       </c>
       <c r="C62" s="1" t="n">
@@ -2490,7 +5446,7 @@
       <c r="A63" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B63" s="22" t="s">
+      <c r="B63" s="21" t="s">
         <v>128</v>
       </c>
       <c r="C63" s="1" t="n">
@@ -2688,7 +5644,7 @@
       <c r="A74" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B74" s="22" t="s">
+      <c r="B74" s="21" t="s">
         <v>127</v>
       </c>
       <c r="C74" s="1" t="n">
@@ -2706,7 +5662,7 @@
       <c r="A75" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B75" s="22" t="s">
+      <c r="B75" s="21" t="s">
         <v>128</v>
       </c>
       <c r="C75" s="1" t="n">
@@ -2904,7 +5860,7 @@
       <c r="A86" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B86" s="22" t="s">
+      <c r="B86" s="21" t="s">
         <v>127</v>
       </c>
       <c r="C86" s="1" t="n">
@@ -2922,7 +5878,7 @@
       <c r="A87" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B87" s="22" t="s">
+      <c r="B87" s="21" t="s">
         <v>128</v>
       </c>
       <c r="C87" s="1" t="n">
@@ -3120,7 +6076,7 @@
       <c r="A98" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B98" s="22" t="s">
+      <c r="B98" s="21" t="s">
         <v>127</v>
       </c>
       <c r="C98" s="1" t="n">
@@ -3138,7 +6094,7 @@
       <c r="A99" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B99" s="22" t="s">
+      <c r="B99" s="21" t="s">
         <v>128</v>
       </c>
       <c r="C99" s="1" t="n">
@@ -3336,7 +6292,7 @@
       <c r="A110" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B110" s="22" t="s">
+      <c r="B110" s="21" t="s">
         <v>127</v>
       </c>
       <c r="C110" s="1" t="n">
@@ -3354,7 +6310,7 @@
       <c r="A111" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B111" s="22" t="s">
+      <c r="B111" s="21" t="s">
         <v>128</v>
       </c>
       <c r="C111" s="1" t="n">
@@ -3552,7 +6508,7 @@
       <c r="A122" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B122" s="22" t="s">
+      <c r="B122" s="21" t="s">
         <v>127</v>
       </c>
       <c r="C122" s="1" t="n">
@@ -3570,7 +6526,7 @@
       <c r="A123" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B123" s="22" t="s">
+      <c r="B123" s="21" t="s">
         <v>128</v>
       </c>
       <c r="C123" s="1" t="n">
@@ -3768,7 +6724,7 @@
       <c r="A134" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B134" s="22" t="s">
+      <c r="B134" s="21" t="s">
         <v>127</v>
       </c>
       <c r="C134" s="1" t="n">
@@ -3786,7 +6742,7 @@
       <c r="A135" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B135" s="22" t="s">
+      <c r="B135" s="21" t="s">
         <v>128</v>
       </c>
       <c r="C135" s="1" t="n">
@@ -3992,7 +6948,7 @@
       <c r="A146" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B146" s="22" t="s">
+      <c r="B146" s="21" t="s">
         <v>127</v>
       </c>
       <c r="C146" s="1" t="n">
@@ -4010,7 +6966,7 @@
       <c r="A147" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B147" s="22" t="s">
+      <c r="B147" s="21" t="s">
         <v>128</v>
       </c>
       <c r="C147" s="1" t="n">
@@ -4208,7 +7164,7 @@
       <c r="A158" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B158" s="22" t="s">
+      <c r="B158" s="21" t="s">
         <v>127</v>
       </c>
       <c r="C158" s="1" t="n">
@@ -4226,7 +7182,7 @@
       <c r="A159" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B159" s="22" t="s">
+      <c r="B159" s="21" t="s">
         <v>128</v>
       </c>
       <c r="C159" s="1" t="n">
@@ -4439,7 +7395,7 @@
   </sheetPr>
   <dimension ref="A1:A49"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
@@ -4674,16 +7630,16 @@
       <c r="C2" s="1" t="n">
         <v>150</v>
       </c>
-      <c r="D2" s="20" t="n">
+      <c r="D2" s="19" t="n">
         <v>45658</v>
       </c>
-      <c r="E2" s="20" t="n">
+      <c r="E2" s="19" t="n">
         <v>46053</v>
       </c>
-      <c r="F2" s="20" t="n">
+      <c r="F2" s="19" t="n">
         <v>45658</v>
       </c>
-      <c r="G2" s="20" t="n">
+      <c r="G2" s="19" t="n">
         <v>46053</v>
       </c>
       <c r="H2" s="1" t="s">
@@ -4709,14 +7665,14 @@
   <dimension ref="A1:F154"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A70" activeCellId="0" sqref="A70"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.57"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="2" style="7" width="11.57"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="11.57"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="6" width="11.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6813,14 +9769,14 @@
   <dimension ref="A1:J150"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="22.71"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.57"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="11.57"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="6" width="11.57"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="17" width="11.57"/>
   </cols>
   <sheetData>
@@ -9191,10 +12147,10 @@
       </c>
     </row>
     <row r="138" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A138" s="19" t="s">
+      <c r="A138" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B138" s="19" t="s">
+      <c r="B138" s="1" t="s">
         <v>70</v>
       </c>
       <c r="C138" s="18" t="n">
@@ -9207,10 +12163,10 @@
       </c>
     </row>
     <row r="139" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A139" s="19" t="s">
+      <c r="A139" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B139" s="19" t="s">
+      <c r="B139" s="1" t="s">
         <v>79</v>
       </c>
       <c r="C139" s="18" t="n">
@@ -9223,10 +12179,10 @@
       </c>
     </row>
     <row r="140" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A140" s="19" t="s">
+      <c r="A140" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B140" s="19" t="s">
+      <c r="B140" s="1" t="s">
         <v>96</v>
       </c>
       <c r="C140" s="18" t="n">
@@ -9239,10 +12195,10 @@
       </c>
     </row>
     <row r="141" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A141" s="19" t="s">
+      <c r="A141" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B141" s="19" t="s">
+      <c r="B141" s="1" t="s">
         <v>105</v>
       </c>
       <c r="C141" s="18" t="n">
@@ -9255,10 +12211,10 @@
       </c>
     </row>
     <row r="142" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A142" s="19" t="s">
+      <c r="A142" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B142" s="19" t="s">
+      <c r="B142" s="1" t="s">
         <v>114</v>
       </c>
       <c r="C142" s="18" t="n">
@@ -9353,296 +12309,296 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C5" s="20"/>
-      <c r="D5" s="20"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C6" s="20"/>
-      <c r="D6" s="20"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C7" s="20"/>
-      <c r="D7" s="20"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C10" s="20"/>
-      <c r="D10" s="20"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C12" s="20"/>
-      <c r="D12" s="20"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C13" s="20"/>
-      <c r="D13" s="20"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C14" s="20"/>
-      <c r="D14" s="20"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C15" s="20"/>
-      <c r="D15" s="20"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C16" s="20"/>
-      <c r="D16" s="20"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C17" s="20"/>
-      <c r="D17" s="20"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C18" s="20"/>
-      <c r="D18" s="20"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C19" s="20"/>
-      <c r="D19" s="20"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C20" s="20"/>
-      <c r="D20" s="20"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="19"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C21" s="20"/>
-      <c r="D21" s="20"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="19"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C22" s="20"/>
-      <c r="D22" s="20"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="19"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C23" s="20"/>
-      <c r="D23" s="20"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="19"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C24" s="20"/>
-      <c r="D24" s="20"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="19"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C25" s="20"/>
-      <c r="D25" s="20"/>
+      <c r="C25" s="19"/>
+      <c r="D25" s="19"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C26" s="20"/>
-      <c r="D26" s="20"/>
+      <c r="C26" s="19"/>
+      <c r="D26" s="19"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C27" s="20"/>
-      <c r="D27" s="20"/>
+      <c r="C27" s="19"/>
+      <c r="D27" s="19"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C28" s="20"/>
-      <c r="D28" s="20"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C29" s="20"/>
-      <c r="D29" s="20"/>
+      <c r="C29" s="19"/>
+      <c r="D29" s="19"/>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C30" s="20"/>
-      <c r="D30" s="20"/>
+      <c r="C30" s="19"/>
+      <c r="D30" s="19"/>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C31" s="20"/>
-      <c r="D31" s="20"/>
+      <c r="C31" s="19"/>
+      <c r="D31" s="19"/>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C32" s="20"/>
-      <c r="D32" s="20"/>
+      <c r="C32" s="19"/>
+      <c r="D32" s="19"/>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C33" s="20"/>
-      <c r="D33" s="20"/>
+      <c r="C33" s="19"/>
+      <c r="D33" s="19"/>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C34" s="20"/>
-      <c r="D34" s="20"/>
+      <c r="C34" s="19"/>
+      <c r="D34" s="19"/>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C35" s="20"/>
-      <c r="D35" s="20"/>
+      <c r="C35" s="19"/>
+      <c r="D35" s="19"/>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C36" s="20"/>
-      <c r="D36" s="20"/>
+      <c r="C36" s="19"/>
+      <c r="D36" s="19"/>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C37" s="20"/>
-      <c r="D37" s="20"/>
+      <c r="C37" s="19"/>
+      <c r="D37" s="19"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C38" s="20"/>
-      <c r="D38" s="20"/>
+      <c r="C38" s="19"/>
+      <c r="D38" s="19"/>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C39" s="20"/>
-      <c r="D39" s="20"/>
+      <c r="C39" s="19"/>
+      <c r="D39" s="19"/>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C40" s="20"/>
-      <c r="D40" s="20"/>
+      <c r="C40" s="19"/>
+      <c r="D40" s="19"/>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
     </row>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C41" s="20"/>
-      <c r="D41" s="20"/>
+      <c r="C41" s="19"/>
+      <c r="D41" s="19"/>
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C42" s="20"/>
-      <c r="D42" s="20"/>
+      <c r="C42" s="19"/>
+      <c r="D42" s="19"/>
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
     </row>
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C43" s="20"/>
-      <c r="D43" s="20"/>
+      <c r="C43" s="19"/>
+      <c r="D43" s="19"/>
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C44" s="20"/>
-      <c r="D44" s="20"/>
+      <c r="C44" s="19"/>
+      <c r="D44" s="19"/>
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
     </row>
     <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C45" s="20"/>
-      <c r="D45" s="20"/>
+      <c r="C45" s="19"/>
+      <c r="D45" s="19"/>
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
     </row>
     <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C46" s="20"/>
-      <c r="D46" s="20"/>
+      <c r="C46" s="19"/>
+      <c r="D46" s="19"/>
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
     </row>
     <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C47" s="20"/>
-      <c r="D47" s="20"/>
+      <c r="C47" s="19"/>
+      <c r="D47" s="19"/>
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>
     </row>
     <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C48" s="20"/>
-      <c r="D48" s="20"/>
+      <c r="C48" s="19"/>
+      <c r="D48" s="19"/>
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
     </row>
     <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C49" s="20"/>
-      <c r="D49" s="20"/>
+      <c r="C49" s="19"/>
+      <c r="D49" s="19"/>
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
     </row>
     <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C50" s="20"/>
-      <c r="D50" s="20"/>
+      <c r="C50" s="19"/>
+      <c r="D50" s="19"/>
       <c r="E50" s="1"/>
       <c r="F50" s="1"/>
     </row>
@@ -9817,8 +12773,8 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
       <c r="E2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10207,26 +13163,26 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="20"/>
-      <c r="C5" s="20"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="19"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
     </row>
@@ -10671,28 +13627,28 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
       <c r="E2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
       <c r="E3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
       <c r="E4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C5" s="20"/>
-      <c r="D5" s="20"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
       <c r="E5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C6" s="20"/>
-      <c r="D6" s="20"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
       <c r="E6" s="1"/>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11061,8 +14017,8 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="16"/>
@@ -11252,24 +14208,24 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="21" t="s">
         <v>127</v>
       </c>
-      <c r="B2" s="23" t="n">
+      <c r="B2" s="22" t="n">
         <v>45637</v>
       </c>
-      <c r="C2" s="23" t="n">
+      <c r="C2" s="22" t="n">
         <v>45672</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="21" t="s">
         <v>128</v>
       </c>
-      <c r="B3" s="23" t="n">
+      <c r="B3" s="22" t="n">
         <v>45673</v>
       </c>
-      <c r="C3" s="23" t="n">
+      <c r="C3" s="22" t="n">
         <v>45701</v>
       </c>
     </row>
@@ -11277,10 +14233,10 @@
       <c r="A4" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="20" t="s">
         <v>130</v>
       </c>
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="20" t="s">
         <v>131</v>
       </c>
     </row>
@@ -11288,10 +14244,10 @@
       <c r="A5" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="20" t="s">
         <v>133</v>
       </c>
-      <c r="C5" s="21" t="s">
+      <c r="C5" s="20" t="s">
         <v>134</v>
       </c>
     </row>
@@ -11299,10 +14255,10 @@
       <c r="A6" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="20" t="s">
         <v>136</v>
       </c>
-      <c r="C6" s="21" t="s">
+      <c r="C6" s="20" t="s">
         <v>137</v>
       </c>
     </row>
@@ -11310,10 +14266,10 @@
       <c r="A7" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B7" s="21" t="s">
+      <c r="B7" s="20" t="s">
         <v>139</v>
       </c>
-      <c r="C7" s="21" t="s">
+      <c r="C7" s="20" t="s">
         <v>140</v>
       </c>
     </row>
@@ -11324,7 +14280,7 @@
       <c r="B8" s="16" t="n">
         <v>45827</v>
       </c>
-      <c r="C8" s="21" t="s">
+      <c r="C8" s="20" t="s">
         <v>142</v>
       </c>
     </row>
@@ -11332,10 +14288,10 @@
       <c r="A9" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="20" t="s">
         <v>144</v>
       </c>
-      <c r="C9" s="21" t="s">
+      <c r="C9" s="20" t="s">
         <v>145</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Set short names to [invoicing periods]
</commit_message>
<xml_diff>
--- a/ampl-data-input-excel/10-PM.Daniel/10-PM.Daniel.xlsx
+++ b/ampl-data-input-excel/10-PM.Daniel/10-PM.Daniel.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="experts" sheetId="1" state="visible" r:id="rId3"/>
@@ -167,7 +167,6 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Valid expert?</t>
         </r>
@@ -180,7 +179,6 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Valid task?</t>
         </r>
@@ -203,7 +201,6 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Valid expert?</t>
         </r>
@@ -216,7 +213,6 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Valid task?</t>
         </r>
@@ -239,7 +235,6 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Valid expert?</t>
         </r>
@@ -262,7 +257,6 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Valid expert?</t>
         </r>
@@ -275,7 +269,6 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Valid task?</t>
         </r>
@@ -298,7 +291,6 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Valid expert?</t>
         </r>
@@ -386,13 +378,13 @@
     <t xml:space="preserve">Upper</t>
   </si>
   <si>
-    <t xml:space="preserve">January.2025</t>
+    <t xml:space="preserve">Jan.25</t>
   </si>
   <si>
-    <t xml:space="preserve">February.2025</t>
+    <t xml:space="preserve">Feb.25</t>
   </si>
   <si>
-    <t xml:space="preserve">March.2025</t>
+    <t xml:space="preserve">Mar.25</t>
   </si>
   <si>
     <t xml:space="preserve">2025-02-14</t>
@@ -401,7 +393,7 @@
     <t xml:space="preserve">2025-03-16</t>
   </si>
   <si>
-    <t xml:space="preserve">April.2025</t>
+    <t xml:space="preserve">Apr.25</t>
   </si>
   <si>
     <t xml:space="preserve">2025-03-17</t>
@@ -410,7 +402,7 @@
     <t xml:space="preserve">2025-04-14</t>
   </si>
   <si>
-    <t xml:space="preserve">May.2025</t>
+    <t xml:space="preserve">May.25</t>
   </si>
   <si>
     <t xml:space="preserve">2025-04-15</t>
@@ -419,7 +411,7 @@
     <t xml:space="preserve">2025-05-18</t>
   </si>
   <si>
-    <t xml:space="preserve">June.2025</t>
+    <t xml:space="preserve">Jun.25</t>
   </si>
   <si>
     <t xml:space="preserve">2025-05-19</t>
@@ -428,13 +420,13 @@
     <t xml:space="preserve">2025-06-18</t>
   </si>
   <si>
-    <t xml:space="preserve">July.2025</t>
+    <t xml:space="preserve">Jul.25</t>
   </si>
   <si>
     <t xml:space="preserve">2025-07-17</t>
   </si>
   <si>
-    <t xml:space="preserve">August.2025</t>
+    <t xml:space="preserve">Aug.25</t>
   </si>
   <si>
     <t xml:space="preserve">2025-07-18</t>
@@ -443,16 +435,16 @@
     <t xml:space="preserve">2025-08-17</t>
   </si>
   <si>
-    <t xml:space="preserve">September.2025</t>
+    <t xml:space="preserve">Sep.25</t>
   </si>
   <si>
-    <t xml:space="preserve">October.2025</t>
+    <t xml:space="preserve">Oct.25</t>
   </si>
   <si>
-    <t xml:space="preserve">November.2025</t>
+    <t xml:space="preserve">Nov.25</t>
   </si>
   <si>
-    <t xml:space="preserve">December.2025</t>
+    <t xml:space="preserve">Dec.25</t>
   </si>
   <si>
     <t xml:space="preserve">Period</t>
@@ -613,7 +605,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -678,7 +670,7 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -690,24 +682,20 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -899,8 +887,8 @@
   </sheetPr>
   <dimension ref="A1:D1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E20" activeCellId="1" sqref="A2:E2 E20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E20" activeCellId="0" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3985,17 +3973,16 @@
   </sheetPr>
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H6" activeCellId="1" sqref="A2:E2 H6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="24" width="13.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="23" width="13.71"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="3" style="7" width="11.57"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="6" width="11.57"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="6" style="19" width="11.57"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="5" style="6" width="11.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4024,7 +4011,7 @@
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="20" t="s">
         <v>25</v>
       </c>
       <c r="C2" s="1" t="n">
@@ -4037,7 +4024,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A2) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F2" s="21" t="b">
+      <c r="F2" s="6" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B2) &gt; 0</f>
         <v>1</v>
       </c>
@@ -4047,7 +4034,7 @@
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="20" t="s">
         <v>26</v>
       </c>
       <c r="C3" s="1" t="n">
@@ -4060,7 +4047,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A3) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F3" s="21" t="n">
+      <c r="F3" s="6" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B3) &gt; 0</f>
         <v>1</v>
       </c>
@@ -4070,7 +4057,7 @@
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="22" t="s">
         <v>27</v>
       </c>
       <c r="C4" s="1" t="n">
@@ -4083,7 +4070,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A4) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F4" s="21" t="n">
+      <c r="F4" s="6" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B4) &gt; 0</f>
         <v>1</v>
       </c>
@@ -4093,7 +4080,7 @@
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="22" t="s">
         <v>30</v>
       </c>
       <c r="C5" s="1" t="n">
@@ -4106,7 +4093,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A5) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F5" s="21" t="n">
+      <c r="F5" s="6" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B5) &gt; 0</f>
         <v>1</v>
       </c>
@@ -4116,7 +4103,7 @@
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="22" t="s">
         <v>33</v>
       </c>
       <c r="C6" s="1" t="n">
@@ -4129,7 +4116,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A6) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F6" s="21" t="n">
+      <c r="F6" s="6" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B6) &gt; 0</f>
         <v>1</v>
       </c>
@@ -4139,7 +4126,7 @@
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="22" t="s">
         <v>36</v>
       </c>
       <c r="C7" s="1" t="n">
@@ -4152,7 +4139,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A7) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F7" s="21" t="n">
+      <c r="F7" s="6" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B7) &gt; 0</f>
         <v>1</v>
       </c>
@@ -4162,7 +4149,7 @@
       <c r="A8" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="22" t="s">
         <v>39</v>
       </c>
       <c r="C8" s="1" t="n">
@@ -4175,7 +4162,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A8) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F8" s="21" t="n">
+      <c r="F8" s="6" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B8) &gt; 0</f>
         <v>1</v>
       </c>
@@ -4185,7 +4172,7 @@
       <c r="A9" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="22" t="s">
         <v>41</v>
       </c>
       <c r="C9" s="1" t="n">
@@ -4198,7 +4185,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A9) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F9" s="21" t="n">
+      <c r="F9" s="6" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B9) &gt; 0</f>
         <v>1</v>
       </c>
@@ -4208,7 +4195,7 @@
       <c r="A10" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="22" t="s">
         <v>44</v>
       </c>
       <c r="C10" s="1" t="n">
@@ -4221,7 +4208,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A10) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F10" s="21" t="n">
+      <c r="F10" s="6" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B10) &gt; 0</f>
         <v>1</v>
       </c>
@@ -4231,7 +4218,7 @@
       <c r="A11" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="22" t="s">
         <v>45</v>
       </c>
       <c r="C11" s="1" t="n">
@@ -4244,7 +4231,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A11) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F11" s="21" t="n">
+      <c r="F11" s="6" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B11) &gt; 0</f>
         <v>1</v>
       </c>
@@ -4254,7 +4241,7 @@
       <c r="A12" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="22" t="s">
         <v>46</v>
       </c>
       <c r="C12" s="1" t="n">
@@ -4267,7 +4254,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A12) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F12" s="21" t="n">
+      <c r="F12" s="6" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B12) &gt; 0</f>
         <v>1</v>
       </c>
@@ -4277,7 +4264,7 @@
       <c r="A13" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="22" t="s">
         <v>47</v>
       </c>
       <c r="C13" s="1" t="n">
@@ -4290,7 +4277,7 @@
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A13) &gt; 0</f>
         <v>1</v>
       </c>
-      <c r="F13" s="21" t="n">
+      <c r="F13" s="6" t="b">
         <f aca="false">COUNTIF('invoicing periods'!$A$2:$A$1000, B13) &gt; 0</f>
         <v>1</v>
       </c>
@@ -4315,8 +4302,8 @@
   </sheetPr>
   <dimension ref="A1:A49"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="1" sqref="A2:E2 A8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4503,8 +4490,8 @@
   </sheetPr>
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:E2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4584,8 +4571,8 @@
   </sheetPr>
   <dimension ref="A1:F65"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="1" sqref="A2:E2 F2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5144,8 +5131,8 @@
   </sheetPr>
   <dimension ref="A1:G1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="A2:E2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5576,8 +5563,8 @@
   </sheetPr>
   <dimension ref="A1:H70"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:E2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6357,8 +6344,8 @@
   </sheetPr>
   <dimension ref="A1:H70"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G1" activeCellId="1" sqref="A2:E2 G1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6762,15 +6749,15 @@
   </sheetPr>
   <dimension ref="A1:F70"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="1" sqref="A2:E2 F2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.21"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="2" style="7" width="11.57"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="6" style="19" width="11.57"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="6" style="6" width="11.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6801,7 +6788,7 @@
       <c r="B2" s="13" t="n">
         <v>45658</v>
       </c>
-      <c r="C2" s="20" t="n">
+      <c r="C2" s="19" t="n">
         <v>46023</v>
       </c>
       <c r="D2" s="7" t="n">
@@ -6810,7 +6797,7 @@
       <c r="E2" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="F2" s="21" t="b">
+      <c r="F2" s="6" t="b">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A2) &gt; 0</f>
         <v>1</v>
       </c>
@@ -7242,8 +7229,8 @@
   </sheetPr>
   <dimension ref="A1:H70"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H1" activeCellId="1" sqref="A2:E2 H1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7252,7 +7239,7 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.57"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="3" style="7" width="11.57"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="11.57"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="7" style="19" width="11.57"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="7" style="6" width="11.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7647,15 +7634,15 @@
   </sheetPr>
   <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:E2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.57"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="2" style="7" width="11.57"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="6" style="19" width="11.57"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="6" style="6" width="11.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7686,7 +7673,7 @@
       <c r="B2" s="13" t="n">
         <v>45658</v>
       </c>
-      <c r="C2" s="20" t="n">
+      <c r="C2" s="19" t="n">
         <v>46023</v>
       </c>
       <c r="D2" s="7" t="n">
@@ -7695,7 +7682,7 @@
       <c r="E2" s="7" t="n">
         <v>3</v>
       </c>
-      <c r="F2" s="21" t="b">
+      <c r="F2" s="6" t="b">
         <f aca="false">COUNTIF(experts!$A$2:$A$987, A2) &gt; 0</f>
         <v>1</v>
       </c>
@@ -7867,8 +7854,8 @@
   </sheetPr>
   <dimension ref="A1:C48"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G29" activeCellId="1" sqref="A2:E2 G29"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7889,95 +7876,95 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="23" t="n">
+      <c r="B2" s="21" t="n">
         <v>45637</v>
       </c>
-      <c r="C2" s="23" t="n">
+      <c r="C2" s="21" t="n">
         <v>45672</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="23" t="n">
+      <c r="B3" s="21" t="n">
         <v>45673</v>
       </c>
-      <c r="C3" s="23" t="n">
+      <c r="C3" s="21" t="n">
         <v>45701</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="20" t="s">
+      <c r="C4" s="19" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="19" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="20" t="s">
+      <c r="B6" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="20" t="s">
+      <c r="C6" s="19" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="20" t="s">
+      <c r="C7" s="19" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="22" t="s">
         <v>39</v>
       </c>
       <c r="B8" s="13" t="n">
         <v>45827</v>
       </c>
-      <c r="C8" s="20" t="s">
+      <c r="C8" s="19" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="B9" s="20" t="s">
+      <c r="B9" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="C9" s="20" t="s">
+      <c r="C9" s="19" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="22" t="s">
         <v>44</v>
       </c>
       <c r="B10" s="13" t="n">
@@ -7988,7 +7975,7 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="22" t="s">
         <v>45</v>
       </c>
       <c r="B11" s="13" t="n">
@@ -7999,7 +7986,7 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="22" t="s">
         <v>46</v>
       </c>
       <c r="B12" s="13" t="n">
@@ -8010,7 +7997,7 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="22" t="s">
         <v>47</v>
       </c>
       <c r="B13" s="13" t="n">

</xml_diff>